<commit_message>
+ em falta: aglomeração 2022
</commit_message>
<xml_diff>
--- a/SAP/CCS_ZPP_IMPORT_OF - Importação de OF's (PULL).xlsx
+++ b/SAP/CCS_ZPP_IMPORT_OF - Importação de OF's (PULL).xlsx
@@ -664,14 +664,14 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>3823001114</v>
+        <v>3820016515</v>
       </c>
       <c r="C3" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>70014930</t>
+          <t>71000843</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -679,11 +679,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ZNRL</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1718.64</v>
+        <v>23</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -693,7 +693,7 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>20211203</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -714,14 +714,14 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3823001114</v>
+        <v>3820016515</v>
       </c>
       <c r="C4" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>70007848</t>
+          <t>71000949</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -729,11 +729,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ZCAC</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1718.64</v>
+        <v>23</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -743,7 +743,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>20220114</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -764,14 +764,14 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3823001114</v>
+        <v>3820016515</v>
       </c>
       <c r="C5" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>70007847</t>
+          <t>71000481</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -779,11 +779,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ZCAC</t>
+          <t>ZRPL</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>168</v>
+        <v>500</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -793,7 +793,7 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>20220114</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
@@ -814,14 +814,14 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>3823001114</v>
+        <v>3823001120</v>
       </c>
       <c r="C6" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>70007846</t>
+          <t>70011415</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -829,11 +829,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ZCEA</t>
+          <t>ZCMQ</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>168</v>
+        <v>400</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -843,7 +843,7 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
-          <t>20220114</t>
+          <t>20211217</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -864,14 +864,14 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>3820016475</v>
+        <v>3823001120</v>
       </c>
       <c r="C7" t="n">
-        <v>180</v>
+        <v>20</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>70000276</t>
+          <t>72000281</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -879,11 +879,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ZNPL</t>
+          <t>ZCMM</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>54</v>
+        <v>400</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -893,7 +893,7 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20211217</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -914,14 +914,14 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>3820016475</v>
+        <v>3823001120</v>
       </c>
       <c r="C8" t="n">
-        <v>180</v>
+        <v>20</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>70000391</t>
+          <t>72000470</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -929,11 +929,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>ZCEQ</t>
+          <t>ZCEM</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>480</v>
+        <v>400</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -943,7 +943,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20211217</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -964,26 +964,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>3820016475</v>
+        <v>3823001120</v>
       </c>
       <c r="C9" t="n">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>70002083</t>
+          <t>70025396</t>
         </is>
       </c>
       <c r="E9" t="n">
         <v>3801</v>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>ZNPL</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
-        <v>54</v>
+        <v>384</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -993,7 +989,7 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20211217</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -1014,26 +1010,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>3820016475</v>
+        <v>3823001120</v>
       </c>
       <c r="C10" t="n">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>70000386</t>
+          <t>70026680</t>
         </is>
       </c>
       <c r="E10" t="n">
         <v>3801</v>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>ZCQE</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
-        <v>480</v>
+        <v>768</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1043,7 +1035,7 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20211217</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -1064,26 +1056,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>3820016475</v>
+        <v>3823001120</v>
       </c>
       <c r="C11" t="n">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>70000031</t>
+          <t>70026679</t>
         </is>
       </c>
       <c r="E11" t="n">
         <v>3801</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>ZNPL</t>
-        </is>
-      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
-        <v>50</v>
+        <v>768</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1093,7 +1081,7 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20211217</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -1114,14 +1102,14 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>3820016475</v>
+        <v>3823001123</v>
       </c>
       <c r="C12" t="n">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>70001656</t>
+          <t>71000923</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -1129,11 +1117,11 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ZCQE</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>348</v>
+        <v>23</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1143,7 +1131,7 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1164,14 +1152,14 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>3820016475</v>
+        <v>3823001123</v>
       </c>
       <c r="C13" t="n">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>70000022</t>
+          <t>71000094</t>
         </is>
       </c>
       <c r="E13" t="n">
@@ -1179,11 +1167,11 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ZNPL</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>206</v>
+        <v>23</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1193,7 +1181,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1214,14 +1202,14 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>3820016475</v>
+        <v>3823001123</v>
       </c>
       <c r="C14" t="n">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>70000996</t>
+          <t>71000430</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -1229,11 +1217,11 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ZCQE</t>
+          <t>ZRPL</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>1440</v>
+        <v>1500</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1243,7 +1231,7 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>20211126</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
@@ -1264,14 +1252,14 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>3820016454</v>
+        <v>3823001123</v>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>70004729</t>
+          <t>71000914</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -1279,11 +1267,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ZNPL</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>624</v>
+        <v>27</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1293,7 +1281,7 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>20211203</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1314,14 +1302,14 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>3820016454</v>
+        <v>3823001123</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>70024563</t>
+          <t>71000073</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -1329,11 +1317,11 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ZCAC</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>624</v>
+        <v>27</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1343,7 +1331,7 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>20211203</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1364,14 +1352,14 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>3820016454</v>
+        <v>3823001123</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>180</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>70024313</t>
+          <t>71000423</t>
         </is>
       </c>
       <c r="E17" t="n">
@@ -1379,11 +1367,11 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ZCMQ</t>
+          <t>ZRPL</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>600</v>
+        <v>2000</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1393,7 +1381,7 @@
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
-          <t>20211203</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1414,14 +1402,14 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3820016454</v>
+        <v>3823001123</v>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>170</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>70023573</t>
+          <t>71000808</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1429,11 +1417,11 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>ZCEM</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>600</v>
+        <v>25</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1443,7 +1431,7 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>20211203</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -1464,14 +1452,14 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>3820016479</v>
+        <v>3823001123</v>
       </c>
       <c r="C19" t="n">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>70003710</t>
+          <t>71000098</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -1479,11 +1467,11 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>ZRPL</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1493,7 +1481,7 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>20220107</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -1514,22 +1502,26 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>3820016479</v>
+        <v>3823001123</v>
       </c>
       <c r="C20" t="n">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>71005271</t>
+          <t>71000544</t>
         </is>
       </c>
       <c r="E20" t="n">
         <v>3801</v>
       </c>
-      <c r="F20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>ZRPL</t>
+        </is>
+      </c>
       <c r="G20" t="n">
-        <v>131</v>
+        <v>2100</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1539,7 +1531,7 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t>20211231</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K20" t="inlineStr"/>
@@ -1560,22 +1552,26 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>3820016479</v>
+        <v>3823001123</v>
       </c>
       <c r="C21" t="n">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>71005270</t>
+          <t>71000908</t>
         </is>
       </c>
       <c r="E21" t="n">
         <v>3801</v>
       </c>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ZRSE</t>
+        </is>
+      </c>
       <c r="G21" t="n">
-        <v>131</v>
+        <v>7</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1585,7 +1581,7 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>20211231</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
@@ -1606,14 +1602,14 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>3820016479</v>
+        <v>3823001123</v>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>70003710</t>
+          <t>71000067</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1621,11 +1617,11 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>ZRPL</t>
+          <t>ZRSE</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1635,7 +1631,7 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>20220107</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -1656,22 +1652,26 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>3820016479</v>
+        <v>3823001123</v>
       </c>
       <c r="C23" t="n">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>71005269</t>
+          <t>71000460</t>
         </is>
       </c>
       <c r="E23" t="n">
         <v>3801</v>
       </c>
-      <c r="F23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>ZRPL</t>
+        </is>
+      </c>
       <c r="G23" t="n">
-        <v>172</v>
+        <v>500</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1681,7 +1681,7 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>20211231</t>
+          <t>20220408</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
@@ -1698,346 +1698,39 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>3820016479</v>
-      </c>
-      <c r="C24" t="n">
-        <v>20</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>71005268</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
-        <v>3801</v>
-      </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="n">
-        <v>172</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>20211231</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N24" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="A24" s="4" t="n"/>
+      <c r="M24" s="4" t="n"/>
+      <c r="N24" s="4" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>3820016479</v>
-      </c>
-      <c r="C25" t="n">
-        <v>10</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>70003710</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>3801</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>ZRPL</t>
-        </is>
-      </c>
-      <c r="G25" t="n">
-        <v>76</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>20220107</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr"/>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N25" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="A25" s="4" t="n"/>
+      <c r="M25" s="4" t="n"/>
+      <c r="N25" s="4" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>3820016479</v>
-      </c>
-      <c r="C26" t="n">
-        <v>10</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>71005267</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>3801</v>
-      </c>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="n">
-        <v>152</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>20220107</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N26" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="A26" s="4" t="n"/>
+      <c r="M26" s="4" t="n"/>
+      <c r="N26" s="4" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>3823001109</v>
-      </c>
-      <c r="C27" t="n">
-        <v>110</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>70004512</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
-        <v>3801</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>ZNPL</t>
-        </is>
-      </c>
-      <c r="G27" t="n">
-        <v>2100</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>20211126</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N27" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="A27" s="4" t="n"/>
+      <c r="M27" s="4" t="n"/>
+      <c r="N27" s="4" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>3823001109</v>
-      </c>
-      <c r="C28" t="n">
-        <v>110</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>70013969</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>3801</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>ZCQE</t>
-        </is>
-      </c>
-      <c r="G28" t="n">
-        <v>4200</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>20211126</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N28" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="A28" s="4" t="n"/>
+      <c r="M28" s="4" t="n"/>
+      <c r="N28" s="4" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>3823001115</v>
-      </c>
-      <c r="C29" t="n">
-        <v>10</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>70009317</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
-        <v>3801</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>ZCMQ</t>
-        </is>
-      </c>
-      <c r="G29" t="n">
-        <v>384</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>20211126</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N29" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="A29" s="4" t="n"/>
+      <c r="M29" s="4" t="n"/>
+      <c r="N29" s="4" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>3823001115</v>
-      </c>
-      <c r="C30" t="n">
-        <v>10</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>70000683</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
-        <v>3801</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>ZCEM</t>
-        </is>
-      </c>
-      <c r="G30" t="n">
-        <v>384</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>20220114</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="N30" s="4" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
+      <c r="A30" s="4" t="n"/>
+      <c r="M30" s="4" t="n"/>
+      <c r="N30" s="4" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="n"/>

</xml_diff>